<commit_message>
Added tour sheets as excel files
</commit_message>
<xml_diff>
--- a/input/input_data/InputData.xlsx
+++ b/input/input_data/InputData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>InputData</t>
   </si>
@@ -33,22 +33,25 @@
     <t>single driving time in seconds</t>
   </si>
   <si>
-    <t>single driving way in meters</t>
-  </si>
-  <si>
     <t>p</t>
   </si>
   <si>
     <t>%</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
     <t>single emptying time in seconds</t>
+  </si>
+  <si>
+    <t>single driving distance in meters</t>
+  </si>
+  <si>
+    <t>number of iterations</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>meters</t>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -118,6 +121,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -412,17 +416,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.88671875" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -438,7 +442,7 @@
         <v>40</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -449,7 +453,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -460,18 +464,18 @@
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>37</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -482,18 +486,26 @@
         <v>102</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>421</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="B9" s="6">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added function for generating .tsp file for ACO Algorithm testrun
.tsp file automatically generated in the output folder
- needs to be tested
</commit_message>
<xml_diff>
--- a/input/input_data/InputData.xlsx
+++ b/input/input_data/InputData.xlsx
@@ -419,7 +419,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -439,7 +439,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>5</v>
@@ -450,7 +450,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>6</v>
@@ -461,7 +461,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>6</v>
@@ -505,7 +505,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="6">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>